<commit_message>
EPBDS: added the following options to global level configuration: wildcard, trim strings, map nulls, map empty strings, required fields; added the following options to class mapping level configuration: wildcard, trim strings, map nulls, map empty strings, required fields; added the following options to field mapping level configuration: trim strings.
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/index/DeepMappingWithArrayTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/index/DeepMappingWithArrayTest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>classA</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t>org.openl.rules.mapping.to.containers</t>
+  </si>
+  <si>
+    <t>Data GlobalConfiguration globalConfiguration</t>
+  </si>
+  <si>
+    <t>wildcard</t>
+  </si>
+  <si>
+    <t>Wildcard</t>
   </si>
 </sst>
 </file>
@@ -127,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -159,11 +168,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -181,6 +201,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D2:G15"/>
+  <dimension ref="D2:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E5"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -487,16 +508,17 @@
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="12" max="12" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:7">
+    <row r="2" spans="4:12">
       <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="4:7">
+    <row r="3" spans="4:12">
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
@@ -504,27 +526,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="4:7">
+    <row r="4" spans="4:12">
       <c r="D4" s="4"/>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="4:7">
+    <row r="5" spans="4:12">
       <c r="D5" s="4"/>
       <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="4:7">
+    <row r="10" spans="4:12">
       <c r="D10" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="4:7">
+      <c r="L10" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12">
       <c r="D11" s="2" t="s">
         <v>0</v>
       </c>
@@ -537,8 +562,11 @@
       <c r="G11" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="4:7">
+      <c r="L11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="4:12">
       <c r="D12" s="3" t="s">
         <v>11</v>
       </c>
@@ -551,8 +579,11 @@
       <c r="G12" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="4:7">
+      <c r="L12" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="4:12">
       <c r="D13" t="s">
         <v>16</v>
       </c>
@@ -565,8 +596,11 @@
       <c r="G13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="4:7">
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:12">
       <c r="D14" t="s">
         <v>16</v>
       </c>
@@ -580,7 +614,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="4:7">
+    <row r="15" spans="4:12">
       <c r="D15" t="s">
         <v>16</v>
       </c>

</xml_diff>